<commit_message>
Ton message de commit
</commit_message>
<xml_diff>
--- a/bd_fournisseurs_fictif.xlsx
+++ b/bd_fournisseurs_fictif.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3011,6 +3011,55 @@
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ass</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ass</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>ass</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2000 - Caisse - </t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>1402 - Intitulé du compte - 14</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>0.0 (%)</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>